<commit_message>
Enhance TikTok Search Tool with detailed debug logging, improved visibility settings, and dynamic content loading adjustments. Added a new debug search script and README for user guidance.
</commit_message>
<xml_diff>
--- a/tiktok_search_funny_cats.xlsx
+++ b/tiktok_search_funny_cats.xlsx
@@ -422,9 +422,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="50" customWidth="1" min="1" max="1"/>
-    <col width="26" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
-    <col width="36" customWidth="1" min="4" max="4"/>
+    <col width="33" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -458,22 +458,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@super.cute.cat.videos/video/7543269164631297302</t>
+          <t>https://www.tiktok.com/@funnycats.520/video/7542217212543929622</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>super.cute.cat.videos</t>
+          <t>funnycats.520</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7543269164631297302</t>
+          <t>7542217212543929622</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Video by @super.cute.cat.videos</t>
+          <t>Video by @funnycats.520</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -485,22 +485,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@quittycat4/video/7544159262751182136</t>
+          <t>https://www.tiktok.com/@super.cute.cat.videos/video/7543269164631297302</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>quittycat4</t>
+          <t>super.cute.cat.videos</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>7544159262751182136</t>
+          <t>7543269164631297302</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Video by @quittycat4</t>
+          <t>Video by @super.cute.cat.videos</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -512,22 +512,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@super.cute.cat.videos/video/7543978846354263318</t>
+          <t>https://www.tiktok.com/@quittycat4/video/7544159262751182136</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>super.cute.cat.videos</t>
+          <t>quittycat4</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7543978846354263318</t>
+          <t>7544159262751182136</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Video by @super.cute.cat.videos</t>
+          <t>Video by @quittycat4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -539,22 +539,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@catutucom/video/7543337508155804935</t>
+          <t>https://www.tiktok.com/@venishaholden/video/7543203054783384846</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>catutucom</t>
+          <t>venishaholden</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7543337508155804935</t>
+          <t>7543203054783384846</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Video by @catutucom</t>
+          <t>Video by @venishaholden</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -566,22 +566,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@funnycats.520/video/7542217212543929622</t>
+          <t>https://www.tiktok.com/@funny.pets926/video/7542470030911393054</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>funnycats.520</t>
+          <t>funny.pets926</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7542217212543929622</t>
+          <t>7542470030911393054</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Video by @funnycats.520</t>
+          <t>Video by @funny.pets926</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -593,22 +593,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@shadow.the.house.panther/video/7543722299795475734</t>
+          <t>https://www.tiktok.com/@super.cute.cat.videos/video/7543978846354263318</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>shadow.the.house.panther</t>
+          <t>super.cute.cat.videos</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7543722299795475734</t>
+          <t>7543978846354263318</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Video by @shadow.the.house.panther</t>
+          <t>Video by @super.cute.cat.videos</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">

</xml_diff>